<commit_message>
added setters to class
</commit_message>
<xml_diff>
--- a/PFOax_GRAV.xlsx
+++ b/PFOax_GRAV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POTENCIALES\Documents\PRACTICAS\Practicas Profesionales\PF Pochutla, Oax\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\japha\OneDrive\Documentos\GitHub\GravPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25B7040-5AA7-48EE-B228-DA6861F03566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167BCCE4-D896-4E5A-B9A5-BD32C240DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E5AFB7BF-6531-4614-8367-B93BF7DCFC20}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,10 +655,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -984,6 +982,7 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1043,16 +1042,16 @@
       <c r="C2" s="24">
         <v>1779338.7180000001</v>
       </c>
-      <c r="D2" s="41">
+      <c r="D2" s="40">
         <v>16.079122900000002</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="40">
         <v>-96.473552499999997</v>
       </c>
       <c r="F2" s="24">
         <v>2208.85</v>
       </c>
-      <c r="G2" s="42">
+      <c r="G2" s="41">
         <v>2207.9119999999998</v>
       </c>
       <c r="H2" s="1"/>
@@ -1322,13 +1321,13 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="42">
         <v>767472</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="42">
         <v>1767496.3333333333</v>
       </c>
       <c r="D13" s="28">
@@ -1347,13 +1346,13 @@
       <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="42">
         <v>768536.33333333337</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="42">
         <v>1768030</v>
       </c>
       <c r="D14" s="28">
@@ -1368,7 +1367,6 @@
       <c r="G14" s="29">
         <v>1297.3333333333333</v>
       </c>
-      <c r="H14" s="40"/>
       <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2149,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3BD539-7DB9-4857-B28E-A640309A95AF}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>